<commit_message>
Added Test Configuration API and another Tables.
</commit_message>
<xml_diff>
--- a/Docs/TS-DB Design.xlsx
+++ b/Docs/TS-DB Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Test</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Fields to Add/Add Button/Update Button</t>
+  </si>
+  <si>
+    <t>TestArchive</t>
   </si>
 </sst>
 </file>
@@ -320,10 +323,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -635,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -648,11 +651,11 @@
     <col min="4" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -675,13 +678,16 @@
         <v>0</v>
       </c>
       <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -703,14 +709,14 @@
       <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
       <c r="I3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -732,14 +738,14 @@
       <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
       <c r="I4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -755,14 +761,11 @@
       <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:10">
       <c r="C6" t="s">
         <v>12</v>
       </c>
@@ -772,11 +775,11 @@
       <c r="G6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="C7" t="s">
         <v>7</v>
       </c>
@@ -787,7 +790,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="C8" t="s">
         <v>13</v>
       </c>
@@ -795,7 +798,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="C9" t="s">
         <v>20</v>
       </c>
@@ -803,7 +806,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="C10" t="s">
         <v>33</v>
       </c>
@@ -811,22 +814,25 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
       <c r="F11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="F12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="F13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="F14" t="s">
         <v>34</v>
       </c>
@@ -906,10 +912,10 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
       <c r="L4" s="29"/>
-      <c r="M4" s="26" t="s">
+      <c r="M4" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="25"/>
+      <c r="N4" s="26"/>
     </row>
     <row r="5" spans="1:14">
       <c r="C5" s="21"/>
@@ -1295,10 +1301,10 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
       <c r="L4" s="29"/>
-      <c r="M4" s="26" t="s">
+      <c r="M4" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="25"/>
+      <c r="N4" s="26"/>
     </row>
     <row r="5" spans="1:14">
       <c r="C5" s="21"/>
@@ -1615,7 +1621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>

</xml_diff>

<commit_message>
Sachin :Test Series crud
</commit_message>
<xml_diff>
--- a/Docs/TS-DB Design.xlsx
+++ b/Docs/TS-DB Design.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t>Test</t>
   </si>
@@ -152,16 +152,62 @@
   </si>
   <si>
     <t>TestArchive</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>SecurityQuestion</t>
+  </si>
+  <si>
+    <t>SecurityAnswer</t>
+  </si>
+  <si>
+    <t>TestSeries</t>
+  </si>
+  <si>
+    <t>TestSeriesID</t>
+  </si>
+  <si>
+    <t>TestConfigurationID</t>
+  </si>
+  <si>
+    <t>TestSeriesTests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -344,6 +390,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -653,192 +701,397 @@
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15.140625" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+      <c r="K1" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+      <c r="K3" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
+      <c r="K4" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" s="5"/>
+      <c r="I5" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="C6" t="s">
+      <c r="J5" s="6"/>
+      <c r="K5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="C7" t="s">
+      <c r="J6" s="6"/>
+      <c r="K6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="33" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="C8" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="C9" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F9" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="C10" t="s">
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F10" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="C11" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F11" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="F12" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="F13" t="s">
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="F14" t="s">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -846,7 +1099,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:N3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>

</xml_diff>

<commit_message>
Sachin: User Registration done. started Login. API completed.
</commit_message>
<xml_diff>
--- a/Docs/TS-DB Design.xlsx
+++ b/Docs/TS-DB Design.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
   <si>
     <t>Test</t>
   </si>
@@ -154,9 +154,6 @@
     <t>TestArchive</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Mobile</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -191,6 +185,48 @@
   </si>
   <si>
     <t>TestSeriesTests</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>UserTestSerieses</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>UserRoles</t>
+  </si>
+  <si>
+    <t>UserProfile</t>
+  </si>
+  <si>
+    <t>RoleID</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>GroupMembers</t>
+  </si>
+  <si>
+    <t>GroupID</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>District</t>
   </si>
 </sst>
 </file>
@@ -324,6 +360,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -390,8 +428,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,11 +771,11 @@
       <c r="J1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>57</v>
+      <c r="K1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -783,10 +819,10 @@
       <c r="J3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -819,11 +855,11 @@
       <c r="J4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="32" t="s">
-        <v>55</v>
+      <c r="L4" s="10" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -841,7 +877,7 @@
       <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="5"/>
@@ -849,17 +885,17 @@
         <v>18</v>
       </c>
       <c r="J5" s="6"/>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="5"/>
@@ -867,7 +903,7 @@
       <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="5"/>
@@ -875,7 +911,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="6"/>
-      <c r="K6" s="32" t="s">
+      <c r="K6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="L6" s="5" t="s">
@@ -893,14 +929,14 @@
       <c r="F7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="11" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="32" t="s">
-        <v>56</v>
+      <c r="K7" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>11</v>
@@ -909,7 +945,7 @@
     <row r="8" spans="1:12">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="5"/>
@@ -921,14 +957,14 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="32" t="s">
+      <c r="K8" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="5"/>
@@ -1039,54 +1075,122 @@
       <c r="I16" s="8"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>53</v>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1109,368 +1213,368 @@
       <c r="A1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="20"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="19" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="25" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="26"/>
+      <c r="N4" s="28"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="28"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="19" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="29"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="31"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="30"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="32"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="19" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="29"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="31"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="31"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="33"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="31"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="33"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="30"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="32"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="19" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="29"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="31"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="31"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="33"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="31"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="33"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="31"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="33"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="31"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="33"/>
     </row>
     <row r="17" spans="3:14">
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="31"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="33"/>
     </row>
     <row r="18" spans="3:14">
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="31"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="33"/>
     </row>
     <row r="19" spans="3:14">
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="31"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="33"/>
     </row>
     <row r="20" spans="3:14">
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="31"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="33"/>
     </row>
     <row r="21" spans="3:14">
-      <c r="C21" s="21"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="31"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="33"/>
     </row>
     <row r="22" spans="3:14">
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="31"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="33"/>
     </row>
     <row r="23" spans="3:14">
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="31"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="33"/>
     </row>
     <row r="24" spans="3:14">
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="31"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="33"/>
     </row>
     <row r="25" spans="3:14">
-      <c r="C25" s="23"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="30"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1498,366 +1602,366 @@
       <c r="A1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="20"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="19" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="25" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="26"/>
+      <c r="N4" s="28"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="28"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="19" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="29"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="31"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="30"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="32"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="19" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="29"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="31"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="31"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="33"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="31"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="33"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="31"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="33"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1">
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="31"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="33"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="31"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="33"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="31"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="33"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="31"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="33"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="31"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="33"/>
     </row>
     <row r="17" spans="3:14">
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="31"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="33"/>
     </row>
     <row r="18" spans="3:14">
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="31"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="33"/>
     </row>
     <row r="19" spans="3:14">
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="31"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="33"/>
     </row>
     <row r="20" spans="3:14">
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="31"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="33"/>
     </row>
     <row r="21" spans="3:14">
-      <c r="C21" s="21"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="31"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="33"/>
     </row>
     <row r="22" spans="3:14">
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="31"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="33"/>
     </row>
     <row r="23" spans="3:14">
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="31"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="33"/>
     </row>
     <row r="24" spans="3:14">
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="31"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="33"/>
     </row>
     <row r="25" spans="3:14">
-      <c r="C25" s="23"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="30"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>